<commit_message>
Queries a and b done, very close with c but tables are gonna need altered to finish it
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\napier-mail.napier.ac.uk\students\School of Computing\User Data\40168766\My Profile\Desktop\Advanced-Database-Systems\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13860" activeTab="2"/>
   </bookViews>
@@ -14,12 +19,11 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="297">
   <si>
     <t>branch</t>
   </si>
@@ -357,12 +361,6 @@
     <t>LO43 7TH</t>
   </si>
   <si>
-    <t>Draiman</t>
-  </si>
-  <si>
-    <t>Gig</t>
-  </si>
-  <si>
     <t>BS11 3AD</t>
   </si>
   <si>
@@ -907,12 +905,21 @@
   </si>
   <si>
     <t>07911911911</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Kerridge</t>
+  </si>
+  <si>
+    <t>Fun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -977,6 +984,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1024,7 +1034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1059,7 +1069,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1393,10 +1403,10 @@
         <v>365</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>46</v>
@@ -1956,7 +1966,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,13 +2046,13 @@
         <v>365</v>
       </c>
       <c r="J2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K2">
         <v>30000</v>
       </c>
       <c r="M2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2074,7 +2084,7 @@
         <v>908</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K3">
         <v>50000</v>
@@ -2085,10 +2095,10 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
@@ -2109,7 +2119,7 @@
         <v>908</v>
       </c>
       <c r="J4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K4">
         <v>50000</v>
@@ -2120,10 +2130,10 @@
         <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>95</v>
@@ -2144,7 +2154,7 @@
         <v>365</v>
       </c>
       <c r="J5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K5">
         <v>35000</v>
@@ -2176,10 +2186,10 @@
         <v>12</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K6">
         <v>50000</v>
@@ -2214,7 +2224,7 @@
         <v>365</v>
       </c>
       <c r="J7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K7">
         <v>30000</v>
@@ -2249,13 +2259,13 @@
         <v>365</v>
       </c>
       <c r="J8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K8">
         <v>40000</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2284,10 +2294,10 @@
         <v>100</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K9">
         <v>40000</v>
@@ -2298,19 +2308,19 @@
         <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>294</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>295</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>296</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G10">
         <v>867</v>
@@ -2319,10 +2329,10 @@
         <v>114</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K10">
         <v>35000</v>
@@ -2333,19 +2343,19 @@
         <v>82</v>
       </c>
       <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
         <v>119</v>
-      </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" t="s">
-        <v>121</v>
       </c>
       <c r="E11" t="s">
         <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G11">
         <v>190</v>
@@ -2354,10 +2364,10 @@
         <v>867</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K11">
         <v>30000</v>
@@ -2368,19 +2378,19 @@
         <v>77</v>
       </c>
       <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
         <v>115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" t="s">
-        <v>117</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G12">
         <v>290</v>
@@ -2392,7 +2402,7 @@
         <v>321</v>
       </c>
       <c r="J12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K12">
         <v>30000</v>
@@ -2403,19 +2413,19 @@
         <v>82</v>
       </c>
       <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" t="s">
         <v>123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" t="s">
-        <v>125</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G13">
         <v>300</v>
@@ -2424,10 +2434,10 @@
         <v>100</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K13">
         <v>40000</v>
@@ -2438,19 +2448,19 @@
         <v>83</v>
       </c>
       <c r="B14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
         <v>127</v>
-      </c>
-      <c r="C14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" t="s">
-        <v>129</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G14">
         <v>998</v>
@@ -2462,7 +2472,7 @@
         <v>321</v>
       </c>
       <c r="J14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K14">
         <v>50000</v>
@@ -2473,19 +2483,19 @@
         <v>77</v>
       </c>
       <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
         <v>131</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>133</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G15">
         <v>777</v>
@@ -2497,7 +2507,7 @@
         <v>888</v>
       </c>
       <c r="J15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K15">
         <v>30000</v>
@@ -2508,19 +2518,19 @@
         <v>83</v>
       </c>
       <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
         <v>135</v>
-      </c>
-      <c r="C16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" t="s">
-        <v>137</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G16">
         <v>118</v>
@@ -2532,7 +2542,7 @@
         <v>888</v>
       </c>
       <c r="J16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K16">
         <v>35000</v>
@@ -2543,13 +2553,13 @@
         <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
         <v>145</v>
-      </c>
-      <c r="D17" t="s">
-        <v>147</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -2564,7 +2574,7 @@
         <v>888</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K17">
         <v>50000</v>
@@ -2588,15 +2598,15 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -2832,7 +2842,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2840,7 +2850,7 @@
         <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>70</v>
@@ -2855,19 +2865,19 @@
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2875,31 +2885,31 @@
         <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2907,31 +2917,31 @@
         <v>83</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2939,34 +2949,34 @@
         <v>82</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H6" s="5">
         <v>6070</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2974,31 +2984,31 @@
         <v>77</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H7" s="5">
         <v>6207</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3006,31 +3016,31 @@
         <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H8" s="5">
         <v>1147</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3038,28 +3048,28 @@
         <v>83</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H9" s="5">
         <v>3020</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3067,31 +3077,31 @@
         <v>83</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3099,34 +3109,34 @@
         <v>82</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H11" s="5">
         <v>1110</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3134,31 +3144,31 @@
         <v>77</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>183</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H12" s="5">
         <v>6262</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3166,31 +3176,31 @@
         <v>83</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H13" s="5">
         <v>1000</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3198,31 +3208,31 @@
         <v>77</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H14" s="5">
         <v>3040</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3230,28 +3240,28 @@
         <v>77</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H15" s="5">
         <v>1968</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3259,31 +3269,31 @@
         <v>77</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H16" s="5">
         <v>3030</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3291,34 +3301,34 @@
         <v>77</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H17" s="5">
         <v>3040</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3326,66 +3336,66 @@
         <v>77</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H18" s="5">
         <v>1312</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3393,31 +3403,31 @@
         <v>77</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H20" s="5">
         <v>8888</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3425,22 +3435,22 @@
         <v>82</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3448,22 +3458,22 @@
         <v>83</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3471,22 +3481,22 @@
         <v>82</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>